<commit_message>
Balance: slowing move speed & shrinking profit
</commit_message>
<xml_diff>
--- a/doc/city_product.xlsx
+++ b/doc/city_product.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="399">
   <si>
     <t>大米</t>
   </si>
@@ -126,39 +126,15 @@
     <t>0/608</t>
   </si>
   <si>
-    <t>12/832</t>
-  </si>
-  <si>
-    <t>32/466</t>
-  </si>
-  <si>
-    <t>38/630</t>
-  </si>
-  <si>
-    <t>50/544</t>
-  </si>
-  <si>
-    <t>5/823</t>
-  </si>
-  <si>
     <t>0/604</t>
   </si>
   <si>
-    <t>23/798</t>
-  </si>
-  <si>
-    <t>11/1450</t>
-  </si>
-  <si>
     <t>0/599</t>
   </si>
   <si>
     <t>0/994</t>
   </si>
   <si>
-    <t>44/542</t>
-  </si>
-  <si>
     <t>0/221</t>
   </si>
   <si>
@@ -168,9 +144,6 @@
     <t>0/3001</t>
   </si>
   <si>
-    <t>50/379</t>
-  </si>
-  <si>
     <t>0/310</t>
   </si>
   <si>
@@ -186,9 +159,6 @@
     <t>0/700</t>
   </si>
   <si>
-    <t>9/1326</t>
-  </si>
-  <si>
     <t>0/993</t>
   </si>
   <si>
@@ -222,9 +192,6 @@
     <t>0/990</t>
   </si>
   <si>
-    <t>8/782</t>
-  </si>
-  <si>
     <t>0/720</t>
   </si>
   <si>
@@ -303,21 +270,6 @@
     <t>0/593</t>
   </si>
   <si>
-    <t>30/283</t>
-  </si>
-  <si>
-    <t>20/487</t>
-  </si>
-  <si>
-    <t>15/820</t>
-  </si>
-  <si>
-    <t>26/782</t>
-  </si>
-  <si>
-    <t>24/793</t>
-  </si>
-  <si>
     <t>0/1688</t>
   </si>
   <si>
@@ -333,102 +285,24 @@
     <t>0/377</t>
   </si>
   <si>
-    <t>36/584</t>
-  </si>
-  <si>
-    <t>36/484</t>
-  </si>
-  <si>
     <t>0/590</t>
   </si>
   <si>
-    <t>47/277</t>
-  </si>
-  <si>
     <t>0/456</t>
   </si>
   <si>
-    <t>20/505</t>
-  </si>
-  <si>
     <t>0/767</t>
   </si>
   <si>
     <t>0/560</t>
   </si>
   <si>
-    <t>23/510</t>
-  </si>
-  <si>
-    <t>18/1290</t>
-  </si>
-  <si>
-    <t>20/1399</t>
-  </si>
-  <si>
-    <t>18/800</t>
-  </si>
-  <si>
-    <t>38/133</t>
-  </si>
-  <si>
-    <t>31/644</t>
-  </si>
-  <si>
     <t>0/473</t>
   </si>
   <si>
     <t>30/560</t>
   </si>
   <si>
-    <t>30/388</t>
-  </si>
-  <si>
-    <t>30/777</t>
-  </si>
-  <si>
-    <t>37/280</t>
-  </si>
-  <si>
-    <t>19/802</t>
-  </si>
-  <si>
-    <t>44/479</t>
-  </si>
-  <si>
-    <t>21/548</t>
-  </si>
-  <si>
-    <t>31/498</t>
-  </si>
-  <si>
-    <t>18/499</t>
-  </si>
-  <si>
-    <t>10/765</t>
-  </si>
-  <si>
-    <t>17/1440</t>
-  </si>
-  <si>
-    <t>16/822</t>
-  </si>
-  <si>
-    <t>42/370</t>
-  </si>
-  <si>
-    <t>25/655</t>
-  </si>
-  <si>
-    <t>28/550</t>
-  </si>
-  <si>
-    <t>40/281</t>
-  </si>
-  <si>
-    <t>22/626</t>
-  </si>
-  <si>
     <t>0/307</t>
   </si>
   <si>
@@ -438,9 +312,6 @@
     <t>0/308</t>
   </si>
   <si>
-    <t>23/391</t>
-  </si>
-  <si>
     <t>0/463</t>
   </si>
   <si>
@@ -456,9 +327,6 @@
     <t>0/469</t>
   </si>
   <si>
-    <t>35/389</t>
-  </si>
-  <si>
     <t>0/975</t>
   </si>
   <si>
@@ -471,15 +339,6 @@
     <t>0/692</t>
   </si>
   <si>
-    <t>26/301</t>
-  </si>
-  <si>
-    <t>19/298</t>
-  </si>
-  <si>
-    <t>20/302</t>
-  </si>
-  <si>
     <t>0/488</t>
   </si>
   <si>
@@ -528,18 +387,12 @@
     <t>0/489</t>
   </si>
   <si>
-    <t>6/830</t>
-  </si>
-  <si>
     <t>0/983</t>
   </si>
   <si>
     <t>0/940</t>
   </si>
   <si>
-    <t>0/920</t>
-  </si>
-  <si>
     <t>0/968</t>
   </si>
   <si>
@@ -621,12 +474,6 @@
     <t>0/359</t>
   </si>
   <si>
-    <t>12/490</t>
-  </si>
-  <si>
-    <t>14/516</t>
-  </si>
-  <si>
     <t>0/620</t>
   </si>
   <si>
@@ -687,18 +534,12 @@
     <t>0/928</t>
   </si>
   <si>
-    <t>25/471</t>
-  </si>
-  <si>
     <t>0/591</t>
   </si>
   <si>
     <t>0/579</t>
   </si>
   <si>
-    <t>0/594</t>
-  </si>
-  <si>
     <t>0/562</t>
   </si>
   <si>
@@ -756,9 +597,6 @@
     <t>0/649</t>
   </si>
   <si>
-    <t>10/1353</t>
-  </si>
-  <si>
     <t>0/1600</t>
   </si>
   <si>
@@ -804,18 +642,12 @@
     <t>0/1547</t>
   </si>
   <si>
-    <t>0/1528</t>
-  </si>
-  <si>
     <t>0/1586</t>
   </si>
   <si>
     <t>0/1576</t>
   </si>
   <si>
-    <t>19/831</t>
-  </si>
-  <si>
     <t>0/998</t>
   </si>
   <si>
@@ -834,15 +666,6 @@
     <t>0/960</t>
   </si>
   <si>
-    <t>20/987</t>
-  </si>
-  <si>
-    <t>27/1020</t>
-  </si>
-  <si>
-    <t>16/1034</t>
-  </si>
-  <si>
     <t>0/1195</t>
   </si>
   <si>
@@ -888,12 +711,6 @@
     <t>0/1233</t>
   </si>
   <si>
-    <t>34/135</t>
-  </si>
-  <si>
-    <t>40/128</t>
-  </si>
-  <si>
     <t>0/154</t>
   </si>
   <si>
@@ -963,12 +780,6 @@
     <t>0/226</t>
   </si>
   <si>
-    <t>40/589</t>
-  </si>
-  <si>
-    <t>24/604</t>
-  </si>
-  <si>
     <t>0/734</t>
   </si>
   <si>
@@ -978,9 +789,6 @@
     <t>0/702</t>
   </si>
   <si>
-    <t>0/749</t>
-  </si>
-  <si>
     <t>0/711</t>
   </si>
   <si>
@@ -1041,15 +849,6 @@
     <t>0/808</t>
   </si>
   <si>
-    <t>6/2457</t>
-  </si>
-  <si>
-    <t>4/2490</t>
-  </si>
-  <si>
-    <t>12/2520</t>
-  </si>
-  <si>
     <t>0/2930</t>
   </si>
   <si>
@@ -1140,9 +939,6 @@
     <t>0/1694</t>
   </si>
   <si>
-    <t>33/389</t>
-  </si>
-  <si>
     <t>0/470</t>
   </si>
   <si>
@@ -1158,9 +954,6 @@
     <t>0/480</t>
   </si>
   <si>
-    <t>24/491</t>
-  </si>
-  <si>
     <t>0/603</t>
   </si>
   <si>
@@ -1210,6 +1003,219 @@
   </si>
   <si>
     <t>0/607</t>
+  </si>
+  <si>
+    <t>30/293</t>
+  </si>
+  <si>
+    <t>47/287</t>
+  </si>
+  <si>
+    <t>37/290</t>
+  </si>
+  <si>
+    <t>40/291</t>
+  </si>
+  <si>
+    <t>23/421</t>
+  </si>
+  <si>
+    <t>5/903</t>
+  </si>
+  <si>
+    <t>8/872</t>
+  </si>
+  <si>
+    <t>6/910</t>
+  </si>
+  <si>
+    <t>10/885</t>
+  </si>
+  <si>
+    <t>20/555</t>
+  </si>
+  <si>
+    <t>23/560</t>
+  </si>
+  <si>
+    <t>31/558</t>
+  </si>
+  <si>
+    <t>26/331</t>
+  </si>
+  <si>
+    <t>19/328</t>
+  </si>
+  <si>
+    <t>20/332</t>
+  </si>
+  <si>
+    <t>12/540</t>
+  </si>
+  <si>
+    <t>14/556</t>
+  </si>
+  <si>
+    <t>12/912</t>
+  </si>
+  <si>
+    <t>24/893</t>
+  </si>
+  <si>
+    <t>16/912</t>
+  </si>
+  <si>
+    <t>32/516</t>
+  </si>
+  <si>
+    <t>34/145</t>
+  </si>
+  <si>
+    <t>38/700</t>
+  </si>
+  <si>
+    <t>23/898</t>
+  </si>
+  <si>
+    <t>6/2757</t>
+  </si>
+  <si>
+    <t>11/1550</t>
+  </si>
+  <si>
+    <t>15/890</t>
+  </si>
+  <si>
+    <t>25/511</t>
+  </si>
+  <si>
+    <t>44/602</t>
+  </si>
+  <si>
+    <t>10/1503</t>
+  </si>
+  <si>
+    <t>20/517</t>
+  </si>
+  <si>
+    <t>9/1526</t>
+  </si>
+  <si>
+    <t>26/882</t>
+  </si>
+  <si>
+    <t>36/604</t>
+  </si>
+  <si>
+    <t>20/1087</t>
+  </si>
+  <si>
+    <t>19/891</t>
+  </si>
+  <si>
+    <t>27/1102</t>
+  </si>
+  <si>
+    <t>40/138</t>
+  </si>
+  <si>
+    <t>36/544</t>
+  </si>
+  <si>
+    <t>50/554</t>
+  </si>
+  <si>
+    <t>4/2790</t>
+  </si>
+  <si>
+    <t>38/143</t>
+  </si>
+  <si>
+    <t>24/654</t>
+  </si>
+  <si>
+    <t>18/900</t>
+  </si>
+  <si>
+    <t>40/649</t>
+  </si>
+  <si>
+    <t>31/704</t>
+  </si>
+  <si>
+    <t>33/439</t>
+  </si>
+  <si>
+    <t>50/439</t>
+  </si>
+  <si>
+    <t>30/438</t>
+  </si>
+  <si>
+    <t>30/887</t>
+  </si>
+  <si>
+    <t>19/892</t>
+  </si>
+  <si>
+    <t>21/618</t>
+  </si>
+  <si>
+    <t>24/541</t>
+  </si>
+  <si>
+    <t>17/1540</t>
+  </si>
+  <si>
+    <t>20/1549</t>
+  </si>
+  <si>
+    <t>18/529</t>
+  </si>
+  <si>
+    <t>12/2720</t>
+  </si>
+  <si>
+    <t>44/539</t>
+  </si>
+  <si>
+    <t>16/1114</t>
+  </si>
+  <si>
+    <t>25/705</t>
+  </si>
+  <si>
+    <t>28/600</t>
+  </si>
+  <si>
+    <t>35/439</t>
+  </si>
+  <si>
+    <t>42/430</t>
+  </si>
+  <si>
+    <t>22/666</t>
+  </si>
+  <si>
+    <t>0/568</t>
+  </si>
+  <si>
+    <t>0/747</t>
+  </si>
+  <si>
+    <t>0/561</t>
+  </si>
+  <si>
+    <t>0/564</t>
+  </si>
+  <si>
+    <t>0/1578</t>
+  </si>
+  <si>
+    <t>18/1520</t>
+  </si>
+  <si>
+    <t>0/729</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1617,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E14" sqref="E14"/>
+      <selection pane="topRight" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1689,286 +1695,286 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>110</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>139</v>
+        <v>332</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="F2" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
       <c r="G2" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>35</v>
+        <v>345</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>36</v>
+        <v>348</v>
       </c>
       <c r="J2" t="s">
-        <v>232</v>
+        <v>179</v>
       </c>
       <c r="K2" t="s">
-        <v>246</v>
+        <v>192</v>
       </c>
       <c r="L2" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
       <c r="M2" t="s">
-        <v>274</v>
+        <v>215</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>289</v>
+        <v>349</v>
       </c>
       <c r="O2" t="s">
-        <v>304</v>
+        <v>243</v>
       </c>
       <c r="P2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>37</v>
+        <v>350</v>
       </c>
       <c r="R2" t="s">
-        <v>343</v>
+        <v>276</v>
       </c>
       <c r="S2" t="s">
-        <v>358</v>
+        <v>291</v>
       </c>
       <c r="T2" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="U2" t="s">
-        <v>227</v>
+        <v>174</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>38</v>
+        <v>367</v>
       </c>
       <c r="W2" t="s">
-        <v>270</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" t="s">
         <v>158</v>
       </c>
-      <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" t="s">
-        <v>202</v>
-      </c>
-      <c r="H3" t="s">
-        <v>209</v>
-      </c>
       <c r="I3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J3" t="s">
-        <v>394</v>
+        <v>325</v>
       </c>
       <c r="K3" t="s">
-        <v>247</v>
+        <v>193</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>41</v>
+        <v>351</v>
       </c>
       <c r="M3" t="s">
-        <v>275</v>
+        <v>216</v>
       </c>
       <c r="N3" t="s">
-        <v>291</v>
+        <v>230</v>
       </c>
       <c r="O3" t="s">
-        <v>305</v>
+        <v>244</v>
       </c>
       <c r="P3" t="s">
-        <v>316</v>
+        <v>253</v>
       </c>
       <c r="Q3" t="s">
-        <v>329</v>
+        <v>265</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>42</v>
+        <v>353</v>
       </c>
       <c r="T3" t="s">
-        <v>374</v>
+        <v>306</v>
       </c>
       <c r="U3" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="V3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>96</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>191</v>
+        <v>142</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>200</v>
+        <v>343</v>
       </c>
       <c r="H4" t="s">
-        <v>210</v>
+        <v>159</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>222</v>
+        <v>355</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>45</v>
+        <v>356</v>
       </c>
       <c r="K4" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="L4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" t="s">
+        <v>217</v>
+      </c>
+      <c r="N4" t="s">
+        <v>231</v>
+      </c>
+      <c r="O4" t="s">
         <v>245</v>
       </c>
-      <c r="L4" t="s">
-        <v>69</v>
-      </c>
-      <c r="M4" t="s">
-        <v>276</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" t="s">
         <v>292</v>
       </c>
-      <c r="O4" t="s">
-        <v>306</v>
-      </c>
-      <c r="P4" t="s">
-        <v>317</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" t="s">
-        <v>48</v>
-      </c>
-      <c r="S4" t="s">
-        <v>359</v>
-      </c>
       <c r="T4" s="4" t="s">
-        <v>49</v>
+        <v>375</v>
       </c>
       <c r="U4" t="s">
-        <v>380</v>
+        <v>311</v>
       </c>
       <c r="V4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="W4" t="s">
-        <v>269</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="J5" t="s">
         <v>180</v>
       </c>
-      <c r="F5" t="s">
-        <v>192</v>
-      </c>
-      <c r="G5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J5" t="s">
-        <v>233</v>
-      </c>
       <c r="K5" s="6" t="s">
-        <v>55</v>
+        <v>359</v>
       </c>
       <c r="L5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="M5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="N5" t="s">
-        <v>293</v>
+        <v>232</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>301</v>
+        <v>240</v>
       </c>
       <c r="P5" t="s">
-        <v>318</v>
+        <v>255</v>
       </c>
       <c r="Q5" t="s">
-        <v>330</v>
+        <v>266</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="S5" t="s">
-        <v>358</v>
+        <v>291</v>
       </c>
       <c r="T5" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="U5" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="V5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>97</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -1976,212 +1982,212 @@
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>94</v>
+        <v>328</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="E6" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="F6" t="s">
-        <v>193</v>
+        <v>144</v>
       </c>
       <c r="G6" t="s">
-        <v>203</v>
+        <v>152</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>98</v>
+        <v>346</v>
       </c>
       <c r="I6" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
       <c r="J6" t="s">
-        <v>149</v>
+        <v>105</v>
       </c>
       <c r="K6" t="s">
-        <v>248</v>
+        <v>194</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="M6" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="N6" t="s">
-        <v>294</v>
+        <v>233</v>
       </c>
       <c r="O6" t="s">
-        <v>307</v>
+        <v>246</v>
       </c>
       <c r="P6" t="s">
-        <v>319</v>
+        <v>398</v>
       </c>
       <c r="Q6" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="S6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="T6" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="U6" t="s">
-        <v>381</v>
+        <v>312</v>
       </c>
       <c r="V6" t="s">
-        <v>391</v>
+        <v>322</v>
       </c>
       <c r="W6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:23">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>67</v>
+        <v>334</v>
       </c>
       <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="G7" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="K7" t="s">
+        <v>195</v>
+      </c>
+      <c r="L7" t="s">
+        <v>209</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="N7" t="s">
+        <v>234</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="P7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" t="s">
-        <v>204</v>
-      </c>
-      <c r="H7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K7" t="s">
-        <v>249</v>
-      </c>
-      <c r="L7" t="s">
-        <v>265</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="N7" t="s">
-        <v>295</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="P7" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>71</v>
-      </c>
       <c r="R7" t="s">
-        <v>344</v>
+        <v>277</v>
       </c>
       <c r="S7" t="s">
-        <v>360</v>
+        <v>293</v>
       </c>
       <c r="T7" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="U7" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="V7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="W7" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" t="s">
         <v>160</v>
       </c>
-      <c r="C8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E8" t="s">
-        <v>182</v>
-      </c>
-      <c r="F8" t="s">
-        <v>194</v>
-      </c>
-      <c r="G8" t="s">
-        <v>184</v>
-      </c>
-      <c r="H8" t="s">
-        <v>211</v>
-      </c>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>395</v>
+        <v>326</v>
       </c>
       <c r="K8" t="s">
-        <v>250</v>
+        <v>196</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>264</v>
+        <v>363</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>272</v>
+        <v>364</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>290</v>
+        <v>365</v>
       </c>
       <c r="O8" t="s">
-        <v>308</v>
+        <v>247</v>
       </c>
       <c r="P8" t="s">
-        <v>320</v>
+        <v>256</v>
       </c>
       <c r="Q8" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="R8" t="s">
-        <v>345</v>
+        <v>278</v>
       </c>
       <c r="S8" t="s">
-        <v>361</v>
+        <v>294</v>
       </c>
       <c r="T8" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>105</v>
+        <v>366</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>390</v>
+        <v>321</v>
       </c>
       <c r="W8" t="s">
-        <v>384</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -2189,70 +2195,70 @@
         <v>23</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>107</v>
+        <v>329</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>109</v>
+        <v>337</v>
       </c>
       <c r="F9" t="s">
-        <v>195</v>
+        <v>146</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>392</v>
       </c>
       <c r="J9" t="s">
+        <v>181</v>
+      </c>
+      <c r="K9" t="s">
+        <v>197</v>
+      </c>
+      <c r="L9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N9" t="s">
         <v>234</v>
       </c>
-      <c r="K9" t="s">
-        <v>251</v>
-      </c>
-      <c r="L9" t="s">
-        <v>81</v>
-      </c>
-      <c r="M9" t="s">
-        <v>82</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
+        <v>38</v>
+      </c>
+      <c r="P9" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>393</v>
+      </c>
+      <c r="R9" t="s">
+        <v>279</v>
+      </c>
+      <c r="S9" t="s">
         <v>295</v>
       </c>
-      <c r="O9" t="s">
-        <v>46</v>
-      </c>
-      <c r="P9" t="s">
-        <v>321</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>110</v>
-      </c>
-      <c r="R9" t="s">
-        <v>346</v>
-      </c>
-      <c r="S9" t="s">
-        <v>362</v>
-      </c>
       <c r="T9" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="U9" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="V9" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="W9" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -2260,212 +2266,212 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>162</v>
+      </c>
+      <c r="I10" t="s">
         <v>172</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F10" t="s">
-        <v>196</v>
-      </c>
-      <c r="G10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" t="s">
-        <v>213</v>
-      </c>
-      <c r="I10" t="s">
-        <v>224</v>
-      </c>
       <c r="J10" t="s">
-        <v>235</v>
+        <v>182</v>
       </c>
       <c r="K10" t="s">
-        <v>252</v>
+        <v>198</v>
       </c>
       <c r="L10" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="M10" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="N10" t="s">
-        <v>292</v>
+        <v>231</v>
       </c>
       <c r="O10" t="s">
-        <v>309</v>
+        <v>248</v>
       </c>
       <c r="P10" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="Q10" t="s">
-        <v>331</v>
+        <v>267</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>341</v>
+        <v>368</v>
       </c>
       <c r="S10" t="s">
-        <v>363</v>
+        <v>296</v>
       </c>
       <c r="T10" t="s">
-        <v>374</v>
+        <v>306</v>
       </c>
       <c r="U10" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="V10" t="s">
-        <v>380</v>
+        <v>311</v>
       </c>
       <c r="W10" t="s">
-        <v>265</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>169</v>
+        <v>335</v>
       </c>
       <c r="E11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" t="s">
+        <v>395</v>
+      </c>
+      <c r="J11" t="s">
         <v>183</v>
       </c>
-      <c r="F11" t="s">
-        <v>197</v>
-      </c>
-      <c r="G11" t="s">
-        <v>205</v>
-      </c>
-      <c r="H11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I11" t="s">
-        <v>225</v>
-      </c>
-      <c r="J11" t="s">
-        <v>236</v>
-      </c>
       <c r="K11" s="4" t="s">
-        <v>113</v>
+        <v>397</v>
       </c>
       <c r="L11" t="s">
-        <v>266</v>
+        <v>210</v>
       </c>
       <c r="M11" t="s">
-        <v>278</v>
+        <v>219</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>116</v>
+        <v>369</v>
       </c>
       <c r="O11" t="s">
-        <v>310</v>
+        <v>249</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>315</v>
+        <v>370</v>
       </c>
       <c r="Q11" t="s">
-        <v>332</v>
+        <v>268</v>
       </c>
       <c r="R11" t="s">
-        <v>347</v>
+        <v>280</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>114</v>
+        <v>382</v>
       </c>
       <c r="T11" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="U11" t="s">
-        <v>229</v>
+        <v>176</v>
       </c>
       <c r="V11" t="s">
-        <v>203</v>
+        <v>152</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>115</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="G12" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12" t="s">
         <v>173</v>
       </c>
-      <c r="E12" t="s">
+      <c r="J12" t="s">
         <v>184</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G12" t="s">
-        <v>206</v>
-      </c>
-      <c r="H12" t="s">
-        <v>214</v>
-      </c>
-      <c r="I12" t="s">
-        <v>226</v>
-      </c>
-      <c r="J12" t="s">
-        <v>237</v>
-      </c>
       <c r="K12" t="s">
-        <v>253</v>
+        <v>199</v>
       </c>
       <c r="L12" t="s">
-        <v>267</v>
+        <v>211</v>
       </c>
       <c r="M12" t="s">
-        <v>279</v>
+        <v>220</v>
       </c>
       <c r="N12" t="s">
-        <v>291</v>
+        <v>230</v>
       </c>
       <c r="O12" t="s">
-        <v>311</v>
+        <v>250</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>314</v>
+        <v>372</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>117</v>
+        <v>373</v>
       </c>
       <c r="R12" t="s">
-        <v>348</v>
+        <v>281</v>
       </c>
       <c r="S12" t="s">
-        <v>364</v>
+        <v>297</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="U12" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="V12" s="4" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="W12" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -2473,70 +2479,70 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" t="s">
         <v>136</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E13" t="s">
-        <v>185</v>
-      </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="H13" t="s">
-        <v>215</v>
+        <v>164</v>
       </c>
       <c r="I13" t="s">
-        <v>227</v>
+        <v>174</v>
       </c>
       <c r="J13" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="K13" t="s">
-        <v>254</v>
+        <v>200</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>121</v>
+        <v>377</v>
       </c>
       <c r="M13" t="s">
-        <v>280</v>
+        <v>221</v>
       </c>
       <c r="N13" t="s">
-        <v>296</v>
+        <v>235</v>
       </c>
       <c r="O13" t="s">
-        <v>312</v>
+        <v>251</v>
       </c>
       <c r="P13" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="Q13" t="s">
-        <v>333</v>
+        <v>269</v>
       </c>
       <c r="R13" t="s">
-        <v>349</v>
+        <v>282</v>
       </c>
       <c r="S13" t="s">
-        <v>365</v>
+        <v>298</v>
       </c>
       <c r="T13" t="s">
-        <v>375</v>
+        <v>307</v>
       </c>
       <c r="U13" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="V13" t="s">
-        <v>186</v>
+        <v>137</v>
       </c>
       <c r="W13" t="s">
-        <v>385</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -2544,70 +2550,70 @@
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>122</v>
+        <v>330</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>396</v>
+        <v>327</v>
       </c>
       <c r="F14" t="s">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="G14" t="s">
-        <v>186</v>
+        <v>137</v>
       </c>
       <c r="H14" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
       <c r="I14" t="s">
-        <v>228</v>
+        <v>175</v>
       </c>
       <c r="J14" t="s">
-        <v>238</v>
+        <v>185</v>
       </c>
       <c r="K14" t="s">
-        <v>255</v>
+        <v>201</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>123</v>
+        <v>378</v>
       </c>
       <c r="M14" t="s">
-        <v>281</v>
+        <v>222</v>
       </c>
       <c r="N14" t="s">
-        <v>293</v>
+        <v>232</v>
       </c>
       <c r="O14" t="s">
-        <v>310</v>
+        <v>249</v>
       </c>
       <c r="P14" t="s">
-        <v>322</v>
+        <v>258</v>
       </c>
       <c r="Q14" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="R14" t="s">
-        <v>350</v>
+        <v>283</v>
       </c>
       <c r="S14" t="s">
-        <v>366</v>
+        <v>299</v>
       </c>
       <c r="T14" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
       <c r="U14" t="s">
-        <v>382</v>
+        <v>313</v>
       </c>
       <c r="V14" t="s">
-        <v>392</v>
+        <v>323</v>
       </c>
       <c r="W14" t="s">
-        <v>386</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -2615,70 +2621,70 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="E15" t="s">
-        <v>186</v>
+        <v>137</v>
       </c>
       <c r="F15" t="s">
-        <v>198</v>
+        <v>149</v>
       </c>
       <c r="G15" t="s">
-        <v>207</v>
+        <v>156</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="I15" t="s">
-        <v>229</v>
+        <v>176</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>125</v>
+        <v>379</v>
       </c>
       <c r="K15" t="s">
-        <v>256</v>
+        <v>202</v>
       </c>
       <c r="L15" t="s">
-        <v>211</v>
+        <v>160</v>
       </c>
       <c r="M15" t="s">
-        <v>282</v>
+        <v>223</v>
       </c>
       <c r="N15" t="s">
-        <v>295</v>
+        <v>234</v>
       </c>
       <c r="O15" t="s">
-        <v>313</v>
+        <v>252</v>
       </c>
       <c r="P15" t="s">
-        <v>323</v>
+        <v>259</v>
       </c>
       <c r="Q15" t="s">
-        <v>334</v>
+        <v>270</v>
       </c>
       <c r="R15" t="s">
-        <v>351</v>
+        <v>284</v>
       </c>
       <c r="S15" t="s">
-        <v>367</v>
+        <v>300</v>
       </c>
       <c r="T15" t="s">
-        <v>376</v>
+        <v>308</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="V15" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="W15" t="s">
-        <v>387</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -2686,70 +2692,70 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>167</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>126</v>
+        <v>339</v>
       </c>
       <c r="F16" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="G16" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="H16" t="s">
-        <v>217</v>
+        <v>166</v>
       </c>
       <c r="I16" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="J16" t="s">
-        <v>239</v>
+        <v>186</v>
       </c>
       <c r="K16" t="s">
-        <v>257</v>
+        <v>203</v>
       </c>
       <c r="L16" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="M16" t="s">
-        <v>283</v>
+        <v>224</v>
       </c>
       <c r="N16" t="s">
-        <v>297</v>
+        <v>236</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>303</v>
+        <v>242</v>
       </c>
       <c r="P16" t="s">
-        <v>324</v>
+        <v>260</v>
       </c>
       <c r="Q16" t="s">
-        <v>335</v>
+        <v>271</v>
       </c>
       <c r="R16" t="s">
-        <v>352</v>
+        <v>285</v>
       </c>
       <c r="S16" t="s">
-        <v>368</v>
+        <v>301</v>
       </c>
       <c r="T16" t="s">
-        <v>377</v>
+        <v>309</v>
       </c>
       <c r="U16" t="s">
-        <v>223</v>
+        <v>171</v>
       </c>
       <c r="V16" t="s">
         <v>34</v>
       </c>
       <c r="W16" t="s">
-        <v>220</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -2757,141 +2763,141 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="G17" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17" t="s">
+        <v>167</v>
+      </c>
+      <c r="I17" t="s">
+        <v>177</v>
+      </c>
+      <c r="J17" t="s">
+        <v>187</v>
+      </c>
+      <c r="K17" t="s">
+        <v>204</v>
+      </c>
+      <c r="L17" t="s">
+        <v>212</v>
+      </c>
+      <c r="M17" t="s">
+        <v>225</v>
+      </c>
+      <c r="N17" t="s">
+        <v>235</v>
+      </c>
+      <c r="O17" t="s">
+        <v>250</v>
+      </c>
+      <c r="P17" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>272</v>
+      </c>
+      <c r="R17" t="s">
+        <v>286</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="T17" t="s">
+        <v>92</v>
+      </c>
+      <c r="U17" t="s">
         <v>137</v>
       </c>
-      <c r="C17" t="s">
-        <v>143</v>
-      </c>
-      <c r="D17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="G17" t="s">
-        <v>208</v>
-      </c>
-      <c r="H17" t="s">
-        <v>218</v>
-      </c>
-      <c r="I17" t="s">
-        <v>230</v>
-      </c>
-      <c r="J17" t="s">
-        <v>240</v>
-      </c>
-      <c r="K17" t="s">
-        <v>258</v>
-      </c>
-      <c r="L17" t="s">
-        <v>268</v>
-      </c>
-      <c r="M17" t="s">
-        <v>284</v>
-      </c>
-      <c r="N17" t="s">
-        <v>296</v>
-      </c>
-      <c r="O17" t="s">
-        <v>311</v>
-      </c>
-      <c r="P17" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>336</v>
-      </c>
-      <c r="R17" t="s">
-        <v>353</v>
-      </c>
-      <c r="S17" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="T17" t="s">
-        <v>118</v>
-      </c>
-      <c r="U17" t="s">
-        <v>186</v>
-      </c>
       <c r="V17" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="W17" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>128</v>
+        <v>336</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F18" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>201</v>
+        <v>344</v>
       </c>
       <c r="H18" t="s">
-        <v>219</v>
+        <v>168</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>127</v>
+        <v>383</v>
       </c>
       <c r="J18" t="s">
-        <v>241</v>
+        <v>188</v>
       </c>
       <c r="K18" t="s">
-        <v>259</v>
+        <v>205</v>
       </c>
       <c r="L18" t="s">
-        <v>269</v>
+        <v>213</v>
       </c>
       <c r="M18" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="N18" t="s">
-        <v>295</v>
+        <v>234</v>
       </c>
       <c r="O18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="P18" t="s">
-        <v>326</v>
+        <v>262</v>
       </c>
       <c r="Q18" t="s">
-        <v>337</v>
+        <v>273</v>
       </c>
       <c r="R18" s="7" t="s">
-        <v>342</v>
+        <v>384</v>
       </c>
       <c r="S18" t="s">
-        <v>369</v>
+        <v>302</v>
       </c>
       <c r="T18" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="U18" s="4" t="s">
-        <v>124</v>
+        <v>385</v>
       </c>
       <c r="V18" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="W18" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:23">
@@ -2899,70 +2905,70 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="C19" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="D19" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
       <c r="E19" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="F19" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>130</v>
+        <v>347</v>
       </c>
       <c r="I19" t="s">
-        <v>231</v>
+        <v>178</v>
       </c>
       <c r="J19" t="s">
-        <v>242</v>
+        <v>189</v>
       </c>
       <c r="K19" t="s">
-        <v>260</v>
+        <v>206</v>
       </c>
       <c r="L19" t="s">
-        <v>270</v>
+        <v>214</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>273</v>
+        <v>386</v>
       </c>
       <c r="N19" t="s">
-        <v>291</v>
+        <v>230</v>
       </c>
       <c r="O19" t="s">
-        <v>307</v>
+        <v>246</v>
       </c>
       <c r="P19" t="s">
-        <v>237</v>
+        <v>184</v>
       </c>
       <c r="Q19" t="s">
-        <v>338</v>
+        <v>274</v>
       </c>
       <c r="R19" t="s">
-        <v>354</v>
+        <v>287</v>
       </c>
       <c r="S19" t="s">
-        <v>370</v>
+        <v>303</v>
       </c>
       <c r="T19" t="s">
-        <v>378</v>
+        <v>310</v>
       </c>
       <c r="U19" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="V19" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="W19" t="s">
-        <v>388</v>
+        <v>319</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -2970,70 +2976,70 @@
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="E20" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="F20" t="s">
-        <v>199</v>
+        <v>150</v>
       </c>
       <c r="G20" t="s">
-        <v>205</v>
+        <v>154</v>
       </c>
       <c r="H20" t="s">
+        <v>122</v>
+      </c>
+      <c r="I20" t="s">
+        <v>82</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="K20" t="s">
+        <v>396</v>
+      </c>
+      <c r="L20" t="s">
         <v>170</v>
       </c>
-      <c r="I20" t="s">
-        <v>93</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="K20" t="s">
-        <v>261</v>
-      </c>
-      <c r="L20" t="s">
-        <v>221</v>
-      </c>
       <c r="M20" t="s">
-        <v>286</v>
+        <v>227</v>
       </c>
       <c r="N20" t="s">
-        <v>298</v>
+        <v>237</v>
       </c>
       <c r="O20" t="s">
-        <v>313</v>
+        <v>252</v>
       </c>
       <c r="P20" t="s">
-        <v>327</v>
+        <v>263</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>132</v>
+        <v>387</v>
       </c>
       <c r="R20" t="s">
-        <v>355</v>
+        <v>288</v>
       </c>
       <c r="S20" t="s">
-        <v>371</v>
+        <v>304</v>
       </c>
       <c r="T20" t="s">
-        <v>375</v>
+        <v>307</v>
       </c>
       <c r="U20" t="s">
-        <v>383</v>
+        <v>314</v>
       </c>
       <c r="V20" t="s">
-        <v>393</v>
+        <v>324</v>
       </c>
       <c r="W20" t="s">
-        <v>389</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -3041,70 +3047,70 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>145</v>
+        <v>389</v>
       </c>
       <c r="D21" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
       <c r="G21" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="H21" t="s">
-        <v>220</v>
+        <v>169</v>
       </c>
       <c r="I21" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J21" t="s">
-        <v>243</v>
+        <v>190</v>
       </c>
       <c r="K21" t="s">
-        <v>262</v>
+        <v>207</v>
       </c>
       <c r="L21" t="s">
-        <v>214</v>
+        <v>163</v>
       </c>
       <c r="M21" t="s">
-        <v>287</v>
+        <v>228</v>
       </c>
       <c r="N21" t="s">
-        <v>299</v>
+        <v>238</v>
       </c>
       <c r="O21" t="s">
-        <v>308</v>
+        <v>247</v>
       </c>
       <c r="P21" t="s">
-        <v>328</v>
+        <v>264</v>
       </c>
       <c r="Q21" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="R21" t="s">
-        <v>356</v>
+        <v>289</v>
       </c>
       <c r="S21" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>131</v>
+        <v>390</v>
       </c>
       <c r="U21" t="s">
-        <v>224</v>
+        <v>172</v>
       </c>
       <c r="V21" t="s">
-        <v>182</v>
+        <v>133</v>
       </c>
       <c r="W21" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:23">
@@ -3112,70 +3118,70 @@
         <v>33</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>134</v>
+        <v>331</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
       <c r="E22" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="F22" t="s">
-        <v>197</v>
+        <v>148</v>
       </c>
       <c r="G22" t="s">
         <v>34</v>
       </c>
       <c r="H22" t="s">
-        <v>221</v>
+        <v>170</v>
       </c>
       <c r="I22" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="J22" t="s">
-        <v>244</v>
+        <v>191</v>
       </c>
       <c r="K22" t="s">
-        <v>263</v>
+        <v>208</v>
       </c>
       <c r="L22" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="M22" t="s">
-        <v>288</v>
+        <v>229</v>
       </c>
       <c r="N22" t="s">
-        <v>300</v>
+        <v>239</v>
       </c>
       <c r="O22" t="s">
-        <v>312</v>
+        <v>251</v>
       </c>
       <c r="P22" s="4" t="s">
-        <v>135</v>
+        <v>391</v>
       </c>
       <c r="Q22" t="s">
-        <v>339</v>
+        <v>275</v>
       </c>
       <c r="R22" t="s">
-        <v>357</v>
+        <v>290</v>
       </c>
       <c r="S22" t="s">
-        <v>372</v>
+        <v>305</v>
       </c>
       <c r="T22" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="U22" t="s">
-        <v>230</v>
+        <v>177</v>
       </c>
       <c r="V22" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="W22" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>